<commit_message>
All final evaluation results
</commit_message>
<xml_diff>
--- a/evaluation/results/anogan/split_1/test_50_50/evaluation_metrics.xlsx
+++ b/evaluation/results/anogan/split_1/test_50_50/evaluation_metrics.xlsx
@@ -503,34 +503,34 @@
         <v>0.5</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="H2">
-        <v>0.5</v>
+        <v>0.5061650465008627</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>534</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>534</v>
       </c>
       <c r="K2">
-        <v>534</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>534</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -565,13 +565,13 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0.6666666666666666</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>534</v>
@@ -582,13 +582,13 @@
         <v>18</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E3">
         <v>534</v>
@@ -671,10 +671,10 @@
         <v>24</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>534</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -682,10 +682,10 @@
         <v>25</v>
       </c>
       <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>534</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>